<commit_message>
Actualizar productos.xlsx e imagenes
</commit_message>
<xml_diff>
--- a/tienda/productos.xlsx
+++ b/tienda/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9af133bd758b7a26/Documentos/novacenter/tienda/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A468F1E-60E8-41A0-B42D-400FBE21A1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADDFA7E3-87C7-4576-BFDF-CC2027438A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{0020F5D2-7C76-46BE-8CFF-757F44DE82B7}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{DA9A05FB-5485-46B9-BF99-CAD902E182A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3661,7 +3661,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AABA79-2C49-4A04-88F9-2F0AF52598E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1A2B1B-99B9-46A7-B55A-0509F07DE53F}">
   <dimension ref="A1:N618"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -9164,7 +9164,7 @@
         <v>1500</v>
       </c>
       <c r="L132">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M132">
         <v>0</v>
@@ -15329,7 +15329,7 @@
         <v>590.4</v>
       </c>
       <c r="L279">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M279">
         <v>0</v>
@@ -24137,7 +24137,7 @@
         <v>380</v>
       </c>
       <c r="L489">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M489">
         <v>0</v>
@@ -26600,7 +26600,7 @@
         <v>10800</v>
       </c>
       <c r="L549">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M549">
         <v>0</v>

</xml_diff>